<commit_message>
added mount holes and other
</commit_message>
<xml_diff>
--- a/Kicad/BOM.xlsx
+++ b/Kicad/BOM.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkyle\Desktop\AVMeter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkyle\Documents\Electronic Projects\AVMeter\Kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18595EA7-8D67-4248-9402-17AFBD9862F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA2DC25-7EAC-4C44-8252-A4FC4CFA3DAD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{080D718F-E8CE-4329-95EA-9AF3D13E03E1}"/>
+    <workbookView xWindow="29355" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{080D718F-E8CE-4329-95EA-9AF3D13E03E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>datasheet</t>
   </si>
@@ -118,9 +120,6 @@
     <t>330</t>
   </si>
   <si>
-    <t>DIODE</t>
-  </si>
-  <si>
     <t>L7805</t>
   </si>
   <si>
@@ -268,7 +267,13 @@
     <t>https://www.mouser.com/datasheet/2/315/ABA0000C1255-1128316.pdf</t>
   </si>
   <si>
-    <t>this order</t>
+    <t>In Stock</t>
+  </si>
+  <si>
+    <t>1N4448WQ</t>
+  </si>
+  <si>
+    <t>Need</t>
   </si>
 </sst>
 </file>
@@ -313,16 +318,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -516,25 +534,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E0DCAD1-67BB-4E78-8D35-683D75CBC55B}" name="Table1" displayName="Table1" ref="A1:G20" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:G20" xr:uid="{A87B4406-6FD0-4407-9277-016FE7845ED4}"/>
-  <sortState ref="A2:F20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E0DCAD1-67BB-4E78-8D35-683D75CBC55B}" name="Table1" displayName="Table1" ref="A1:H20" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:H20" xr:uid="{A87B4406-6FD0-4407-9277-016FE7845ED4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
     <sortCondition ref="A1:A20"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="15" xr3:uid="{82903B20-3ACE-482D-A62D-533E5998987C}" uniqueName="ref" name="Type">
       <xmlColumnPr mapId="1" xpath="/export/components/comp/@ref" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{2AA955C5-D151-4757-BCC8-9D3B9D43314C}" uniqueName="value" name="value5">
       <xmlColumnPr mapId="1" xpath="/export/components/comp/value" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{E06DC298-3793-4A6C-AB56-B6BF1FD3CCBF}" uniqueName="46" name="quantity" dataDxfId="0"/>
+    <tableColumn id="46" xr3:uid="{E06DC298-3793-4A6C-AB56-B6BF1FD3CCBF}" uniqueName="46" name="quantity" dataDxfId="2"/>
     <tableColumn id="18" xr3:uid="{04DB9F5D-76A5-4066-B84C-CC0BC093389B}" uniqueName="datasheet" name="datasheet">
       <xmlColumnPr mapId="1" xpath="/export/components/comp/datasheet" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="43" xr3:uid="{9380DE1B-B190-4023-AC15-4670CD9075BA}" uniqueName="43" name="mouser/digikey"/>
     <tableColumn id="44" xr3:uid="{5C2A3E4A-2D7A-4D19-B94F-0BF49F0F4ED0}" uniqueName="44" name="last order"/>
-    <tableColumn id="47" xr3:uid="{53FA32E9-1477-4AFF-B12F-E976EA39FCD6}" uniqueName="47" name="this order"/>
+    <tableColumn id="1" xr3:uid="{2E3A2D39-32F0-4835-9DEF-2EA7B0BD37B5}" uniqueName="1" name="In Stock" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B1FC0163-8340-4033-86F2-B330320CEBE5}" uniqueName="2" name="Need" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,129 +858,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7772728-41D4-4B68-A4C9-A3177FC3416F}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="7" width="8" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="3">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="3">
+        <v>17</v>
+      </c>
+      <c r="H3" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="3">
+        <v>14</v>
+      </c>
+      <c r="H4" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="3"/>
+      <c r="H5" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -967,211 +1016,269 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="3">
+        <v>7</v>
+      </c>
+      <c r="H7" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" s="3">
+        <v>50</v>
+      </c>
+      <c r="H8" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G9" s="3">
+        <v>26</v>
+      </c>
+      <c r="H9" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="3">
+        <v>8</v>
+      </c>
+      <c r="H10" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="3">
+        <v>8</v>
+      </c>
+      <c r="H11" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F12">
         <v>6</v>
       </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="3">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="3">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="3">
+        <v>19</v>
+      </c>
+      <c r="H14" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1179,22 +1286,24 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16">
         <v>3</v>
       </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="3"/>
+      <c r="H16" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1202,19 +1311,26 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,19 +1338,26 @@
         <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1242,36 +1365,50 @@
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20">
         <v>3</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <f>Table1[[#This Row],[In Stock]]-Table1[[#This Row],[quantity]]</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1320,4 +1457,16 @@
     <tablePart r:id="rId39"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB443A7-01A8-4B2D-BFFF-EEB3D794BB30}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>